<commit_message>
ready to run model before lab presentation
</commit_message>
<xml_diff>
--- a/scope/Variable Mappings.xlsx
+++ b/scope/Variable Mappings.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="150" windowWidth="7110" windowHeight="7950"/>
+    <workbookView xWindow="10845" yWindow="30" windowWidth="3315" windowHeight="12795"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -986,8 +986,8 @@
   <dimension ref="A1:H75"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A14" sqref="A14"/>
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1943,7 +1943,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B43"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>

</xml_diff>